<commit_message>
Data up to 10m
</commit_message>
<xml_diff>
--- a/dataCollection2.xlsx
+++ b/dataCollection2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-30340" yWindow="0" windowWidth="30340" windowHeight="21120" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,10 +94,10 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$47</c:f>
+              <c:f>Sheet1!$A$2:$A$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>50.0</c:v>
                 </c:pt>
@@ -235,16 +235,85 @@
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>590.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>610.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>630.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>630.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>650.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>670.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>670.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>690.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>710.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>730.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>750.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>770.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>790.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>810.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>830.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>850.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>870.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>890.0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>890.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>910.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>930.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>950.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>970.0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>990.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$47</c:f>
+              <c:f>Sheet1!$B$2:$B$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+                <c:ptCount val="69"/>
                 <c:pt idx="0">
                   <c:v>-64.44</c:v>
                 </c:pt>
@@ -382,6 +451,75 @@
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>-93.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-91.5</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-82.9411764705882</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-84.2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-89.7058823529411</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-87.4444444444444</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-87.88235294117641</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-86.28</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-87.7142857142857</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-88.35294117647059</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-86.9565217391304</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-84.4347826086956</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-84.6666666666666</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-82.52</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-84.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-86.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-86.5714285714285</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-86.5357142857142</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-86.6666666666666</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-87.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-88.17391304347819</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-89.0555555555555</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-90.3636363636363</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-90.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -396,11 +534,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2078417368"/>
-        <c:axId val="2064662728"/>
+        <c:axId val="2083384840"/>
+        <c:axId val="2083381672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2078417368"/>
+        <c:axId val="2083384840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -410,12 +548,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064662728"/>
+        <c:crossAx val="2083381672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2064662728"/>
+        <c:axId val="2083381672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -426,7 +564,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2078417368"/>
+        <c:crossAx val="2083384840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -453,19 +591,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -805,10 +943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B47"/>
+  <dimension ref="A2:B70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1179,6 +1317,190 @@
       </c>
       <c r="B47">
         <v>-93.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48">
+        <v>610</v>
+      </c>
+      <c r="B48">
+        <v>-91.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49">
+        <v>630</v>
+      </c>
+      <c r="B49">
+        <v>-82.941176470588204</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50">
+        <v>630</v>
+      </c>
+      <c r="B50">
+        <v>-84.2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51">
+        <v>650</v>
+      </c>
+      <c r="B51">
+        <v>-89.705882352941103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52">
+        <v>670</v>
+      </c>
+      <c r="B52">
+        <v>-87.4444444444444</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53">
+        <v>670</v>
+      </c>
+      <c r="B53">
+        <v>-87.882352941176407</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54">
+        <v>690</v>
+      </c>
+      <c r="B54">
+        <v>-86.28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55">
+        <v>710</v>
+      </c>
+      <c r="B55">
+        <v>-87.714285714285694</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56">
+        <v>730</v>
+      </c>
+      <c r="B56">
+        <v>-88.352941176470594</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57">
+        <v>750</v>
+      </c>
+      <c r="B57">
+        <v>-86.956521739130395</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58">
+        <v>770</v>
+      </c>
+      <c r="B58">
+        <v>-84.434782608695599</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59">
+        <v>790</v>
+      </c>
+      <c r="B59">
+        <v>-84.6666666666666</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60">
+        <v>810</v>
+      </c>
+      <c r="B60">
+        <v>-82.52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61">
+        <v>830</v>
+      </c>
+      <c r="B61">
+        <v>-84</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62">
+        <v>850</v>
+      </c>
+      <c r="B62">
+        <v>-86</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63">
+        <v>870</v>
+      </c>
+      <c r="B63">
+        <v>-86.571428571428498</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64">
+        <v>890</v>
+      </c>
+      <c r="B64">
+        <v>-86.535714285714207</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65">
+        <v>890</v>
+      </c>
+      <c r="B65">
+        <v>-86.6666666666666</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66">
+        <v>910</v>
+      </c>
+      <c r="B66">
+        <v>-87</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67">
+        <v>930</v>
+      </c>
+      <c r="B67">
+        <v>-88.173913043478194</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68">
+        <v>950</v>
+      </c>
+      <c r="B68">
+        <v>-89.0555555555555</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69">
+        <v>970</v>
+      </c>
+      <c r="B69">
+        <v>-90.363636363636303</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70">
+        <v>990</v>
+      </c>
+      <c r="B70">
+        <v>-90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>